<commit_message>
Update scenarios / levels and growth
</commit_message>
<xml_diff>
--- a/Internal macros/macro_23_test.xlsx
+++ b/Internal macros/macro_23_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub Projects\EBA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub Projects\EBA\Internal macros\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -408,8 +408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,7 +447,7 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -475,7 +475,7 @@
         <v>1E-4</v>
       </c>
       <c r="D10">
-        <v>1E-4</v>
+        <v>-0.33</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -489,7 +489,7 @@
         <v>1E-4</v>
       </c>
       <c r="D11">
-        <v>1E-4</v>
+        <v>-0.33</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -503,7 +503,7 @@
         <v>1E-4</v>
       </c>
       <c r="D12">
-        <v>1E-4</v>
+        <v>-0.33</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -517,7 +517,7 @@
         <v>1E-4</v>
       </c>
       <c r="D13">
-        <v>1E-4</v>
+        <v>-0.33</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -531,7 +531,7 @@
         <v>1E-4</v>
       </c>
       <c r="D14">
-        <v>1E-4</v>
+        <v>-0.31</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -545,7 +545,7 @@
         <v>1E-4</v>
       </c>
       <c r="D15">
-        <v>1E-4</v>
+        <v>-0.31</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -559,7 +559,7 @@
         <v>1E-4</v>
       </c>
       <c r="D16">
-        <v>1E-4</v>
+        <v>-0.31</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -573,7 +573,7 @@
         <v>1E-4</v>
       </c>
       <c r="D17">
-        <v>1E-4</v>
+        <v>-0.31</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -587,7 +587,7 @@
         <v>1E-4</v>
       </c>
       <c r="D18">
-        <v>1E-4</v>
+        <v>-0.31</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -601,7 +601,7 @@
         <v>1E-4</v>
       </c>
       <c r="D19">
-        <v>1E-4</v>
+        <v>-0.31</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -615,7 +615,7 @@
         <v>1E-4</v>
       </c>
       <c r="D20">
-        <v>1E-4</v>
+        <v>-0.31</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -629,7 +629,7 @@
         <v>1E-4</v>
       </c>
       <c r="D21">
-        <v>1E-4</v>
+        <v>-0.31</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -643,7 +643,7 @@
         <v>1E-4</v>
       </c>
       <c r="D22">
-        <v>1E-4</v>
+        <v>-0.31</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -657,7 +657,7 @@
         <v>1E-4</v>
       </c>
       <c r="D23">
-        <v>1E-4</v>
+        <v>-0.31</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -671,7 +671,7 @@
         <v>1E-4</v>
       </c>
       <c r="D24">
-        <v>1E-4</v>
+        <v>-0.31</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -685,7 +685,7 @@
         <v>1E-4</v>
       </c>
       <c r="D25">
-        <v>1E-4</v>
+        <v>-0.31</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -699,7 +699,7 @@
         <v>1E-4</v>
       </c>
       <c r="D26">
-        <v>1E-4</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -713,7 +713,7 @@
         <v>1E-4</v>
       </c>
       <c r="D27">
-        <v>1E-4</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -727,7 +727,7 @@
         <v>1E-4</v>
       </c>
       <c r="D28">
-        <v>1E-4</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -741,7 +741,7 @@
         <v>1E-4</v>
       </c>
       <c r="D29">
-        <v>1E-4</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -755,7 +755,7 @@
         <v>1E-4</v>
       </c>
       <c r="D30">
-        <v>1E-4</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -769,7 +769,7 @@
         <v>1E-4</v>
       </c>
       <c r="D31">
-        <v>1E-4</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -783,7 +783,7 @@
         <v>1E-4</v>
       </c>
       <c r="D32">
-        <v>1E-4</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -797,7 +797,7 @@
         <v>1E-4</v>
       </c>
       <c r="D33">
-        <v>1E-4</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -811,7 +811,7 @@
         <v>1E-4</v>
       </c>
       <c r="D34">
-        <v>1E-4</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -825,7 +825,7 @@
         <v>1E-4</v>
       </c>
       <c r="D35">
-        <v>1E-4</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -839,7 +839,7 @@
         <v>1E-4</v>
       </c>
       <c r="D36">
-        <v>1E-4</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -853,7 +853,7 @@
         <v>1E-4</v>
       </c>
       <c r="D37">
-        <v>1E-4</v>
+        <v>-0.13</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -867,7 +867,7 @@
         <v>1E-4</v>
       </c>
       <c r="D38">
-        <v>1E-4</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -881,7 +881,7 @@
         <v>1E-4</v>
       </c>
       <c r="D39">
-        <v>1E-4</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -895,7 +895,7 @@
         <v>1E-4</v>
       </c>
       <c r="D40">
-        <v>1E-4</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -909,7 +909,7 @@
         <v>1E-4</v>
       </c>
       <c r="D41">
-        <v>1E-4</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -923,7 +923,7 @@
         <v>1E-4</v>
       </c>
       <c r="D42">
-        <v>1E-4</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -937,7 +937,7 @@
         <v>1E-4</v>
       </c>
       <c r="D43">
-        <v>1E-4</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -951,7 +951,7 @@
         <v>1E-4</v>
       </c>
       <c r="D44">
-        <v>1E-4</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -965,7 +965,7 @@
         <v>1E-4</v>
       </c>
       <c r="D45">
-        <v>1E-4</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -979,7 +979,7 @@
         <v>1E-4</v>
       </c>
       <c r="D46">
-        <v>1E-4</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -993,7 +993,7 @@
         <v>1E-4</v>
       </c>
       <c r="D47">
-        <v>1E-4</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1007,7 +1007,7 @@
         <v>1E-4</v>
       </c>
       <c r="D48">
-        <v>1E-4</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1021,7 +1021,7 @@
         <v>1E-4</v>
       </c>
       <c r="D49">
-        <v>1E-4</v>
+        <v>0.15</v>
       </c>
     </row>
   </sheetData>
@@ -1034,7 +1034,7 @@
   <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D46"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,7 +1084,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>1E-4</v>
+        <v>-0.33</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1098,7 +1098,7 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>1E-4</v>
+        <v>-0.33</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1112,7 +1112,7 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>1E-4</v>
+        <v>-0.33</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1126,7 +1126,7 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>1E-4</v>
+        <v>-0.33</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1140,7 +1140,7 @@
         <v>-3.18</v>
       </c>
       <c r="D11">
-        <v>1E-4</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1154,7 +1154,7 @@
         <v>-3.18</v>
       </c>
       <c r="D12">
-        <v>1E-4</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1168,7 +1168,7 @@
         <v>-3.18</v>
       </c>
       <c r="D13">
-        <v>1E-4</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1182,7 +1182,7 @@
         <v>-3.18</v>
       </c>
       <c r="D14">
-        <v>1E-4</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1196,7 +1196,7 @@
         <v>-3.18</v>
       </c>
       <c r="D15">
-        <v>1E-4</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1210,7 +1210,7 @@
         <v>-3.18</v>
       </c>
       <c r="D16">
-        <v>1E-4</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1224,7 +1224,7 @@
         <v>-3.18</v>
       </c>
       <c r="D17">
-        <v>1E-4</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1238,7 +1238,7 @@
         <v>-3.18</v>
       </c>
       <c r="D18">
-        <v>1E-4</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1252,7 +1252,7 @@
         <v>-3.18</v>
       </c>
       <c r="D19">
-        <v>1E-4</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1266,7 +1266,7 @@
         <v>-3.18</v>
       </c>
       <c r="D20">
-        <v>1E-4</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1280,7 +1280,7 @@
         <v>-3.18</v>
       </c>
       <c r="D21">
-        <v>1E-4</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1294,7 +1294,7 @@
         <v>-3.18</v>
       </c>
       <c r="D22">
-        <v>1E-4</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1308,7 +1308,7 @@
         <v>0.33800000000000002</v>
       </c>
       <c r="D23">
-        <v>1E-4</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1322,7 +1322,7 @@
         <v>0.33800000000000002</v>
       </c>
       <c r="D24">
-        <v>1E-4</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1336,7 +1336,7 @@
         <v>0.33800000000000002</v>
       </c>
       <c r="D25">
-        <v>1E-4</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1350,7 +1350,7 @@
         <v>0.33800000000000002</v>
       </c>
       <c r="D26">
-        <v>1E-4</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1364,7 +1364,7 @@
         <v>0.33800000000000002</v>
       </c>
       <c r="D27">
-        <v>1E-4</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1378,7 +1378,7 @@
         <v>0.33800000000000002</v>
       </c>
       <c r="D28">
-        <v>1E-4</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1392,7 +1392,7 @@
         <v>0.33800000000000002</v>
       </c>
       <c r="D29">
-        <v>1E-4</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1406,7 +1406,7 @@
         <v>0.33800000000000002</v>
       </c>
       <c r="D30">
-        <v>1E-4</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1420,7 +1420,7 @@
         <v>0.33800000000000002</v>
       </c>
       <c r="D31">
-        <v>1E-4</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1434,7 +1434,7 @@
         <v>0.33800000000000002</v>
       </c>
       <c r="D32">
-        <v>1E-4</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1448,7 +1448,7 @@
         <v>0.33800000000000002</v>
       </c>
       <c r="D33">
-        <v>1E-4</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1462,7 +1462,7 @@
         <v>0.33800000000000002</v>
       </c>
       <c r="D34">
-        <v>1E-4</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1476,7 +1476,7 @@
         <v>0.70399999999999996</v>
       </c>
       <c r="D35">
-        <v>1E-4</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1490,7 +1490,7 @@
         <v>0.70399999999999996</v>
       </c>
       <c r="D36">
-        <v>1E-4</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1504,7 +1504,7 @@
         <v>0.70399999999999996</v>
       </c>
       <c r="D37">
-        <v>1E-4</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1518,7 +1518,7 @@
         <v>0.70399999999999996</v>
       </c>
       <c r="D38">
-        <v>1E-4</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1532,7 +1532,7 @@
         <v>0.70399999999999996</v>
       </c>
       <c r="D39">
-        <v>1E-4</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1546,7 +1546,7 @@
         <v>0.70399999999999996</v>
       </c>
       <c r="D40">
-        <v>1E-4</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1560,7 +1560,7 @@
         <v>0.70399999999999996</v>
       </c>
       <c r="D41">
-        <v>1E-4</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1574,7 +1574,7 @@
         <v>0.70399999999999996</v>
       </c>
       <c r="D42">
-        <v>1E-4</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1588,7 +1588,7 @@
         <v>0.70399999999999996</v>
       </c>
       <c r="D43">
-        <v>1E-4</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1602,7 +1602,7 @@
         <v>0.70399999999999996</v>
       </c>
       <c r="D44">
-        <v>1E-4</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1616,7 +1616,7 @@
         <v>0.70399999999999996</v>
       </c>
       <c r="D45">
-        <v>1E-4</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1630,7 +1630,7 @@
         <v>0.70399999999999996</v>
       </c>
       <c r="D46">
-        <v>1E-4</v>
+        <v>0.54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>